<commit_message>
update positive case register
</commit_message>
<xml_diff>
--- a/Resources/testDataCermati.xlsx
+++ b/Resources/testDataCermati.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cermati\cermati\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13AABD5-737A-4DCC-97B9-E30797766EFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C459CC48-AD3A-4233-8014-32B0CF1536D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7185" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{41FE7F68-FC3F-4E35-86F8-BD74FAC7F8A1}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>email</t>
   </si>
@@ -54,9 +54,6 @@
     <t>city</t>
   </si>
   <si>
-    <t>rianfati@gmail.com</t>
-  </si>
-  <si>
     <t>rhaeBpqKT1cvcnbZpSXfmw==</t>
   </si>
   <si>
@@ -66,28 +63,19 @@
     <t>Agusta</t>
   </si>
   <si>
-    <t>081322762669</t>
-  </si>
-  <si>
     <t>Bogor</t>
   </si>
   <si>
-    <t>rianfati</t>
-  </si>
-  <si>
-    <t>rianfati@</t>
-  </si>
-  <si>
-    <t>rianfati.com</t>
-  </si>
-  <si>
-    <t>model</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>0</t>
+    <t>note</t>
+  </si>
+  <si>
+    <t>087765409435</t>
+  </si>
+  <si>
+    <t>rianfati92@gmail.com</t>
+  </si>
+  <si>
+    <t>positive case</t>
   </si>
 </sst>
 </file>
@@ -132,10 +120,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -451,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDCD7E8F-5AAD-4E11-A732-40EFC8018D22}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,6 +458,7 @@
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" customWidth="1"/>
     <col min="6" max="6" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -490,163 +484,38 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1" xr:uid="{AF0E480E-A86A-4056-944A-9A526CCF2699}"/>
-    <hyperlink ref="A7" r:id="rId2" display="rianfati@" xr:uid="{94006596-A56C-4230-9AB9-3EEF5146367C}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BF40F5E5-2010-4E7D-BC0C-6AD6FADD25EF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>